<commit_message>
update of ms figures
</commit_message>
<xml_diff>
--- a/param-values/soil-model-param.xlsx
+++ b/param-values/soil-model-param.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10512"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10928"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/zobitz/Desktop/Finland Projects/FireGrow/param-values/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A2C485AE-BB5B-A043-9DBF-B82DFE3BC2D6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3B1B17A1-39B5-FC46-B11A-5141798F25E7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2480" yWindow="1220" windowWidth="23100" windowHeight="15220" xr2:uid="{DDBE217D-BCD3-DF40-8568-416F7629FDB0}"/>
   </bookViews>
@@ -355,13 +355,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -680,7 +681,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="3" topLeftCell="D1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="K22" sqref="K22"/>
+      <selection pane="topRight" activeCell="I21" sqref="I21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1379,8 +1380,8 @@
       <c r="H18" t="b">
         <v>0</v>
       </c>
-      <c r="I18" s="4" t="b">
-        <v>1</v>
+      <c r="I18" s="6" t="b">
+        <v>0</v>
       </c>
       <c r="J18">
         <v>0</v>
@@ -1531,8 +1532,8 @@
       <c r="H22" t="b">
         <v>1</v>
       </c>
-      <c r="I22" s="4" t="b">
-        <v>1</v>
+      <c r="I22" s="6" t="b">
+        <v>0</v>
       </c>
       <c r="J22">
         <v>0</v>
@@ -1569,8 +1570,8 @@
       <c r="H23" t="b">
         <v>1</v>
       </c>
-      <c r="I23" s="4" t="b">
-        <v>1</v>
+      <c r="I23" s="6" t="b">
+        <v>0</v>
       </c>
       <c r="J23">
         <v>0</v>
@@ -1607,8 +1608,8 @@
       <c r="H24" t="b">
         <v>1</v>
       </c>
-      <c r="I24" s="4" t="b">
-        <v>1</v>
+      <c r="I24" s="6" t="b">
+        <v>0</v>
       </c>
       <c r="J24">
         <v>0</v>

</xml_diff>